<commit_message>
ka cs 6 7
</commit_message>
<xml_diff>
--- a/rill-analysis/rill-analysis-report/src/test/resources/ka-cs-pie-7.xlsx
+++ b/rill-analysis/rill-analysis-report/src/test/resources/ka-cs-pie-7.xlsx
@@ -174,15 +174,15 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>dataType</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>custId</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>ims/cs/diy/cust/pieChart.action</t>
+  </si>
+  <si>
+    <t>dateType</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1222,10 +1222,10 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1" t="s">
@@ -1267,10 +1267,10 @@
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="6" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C12" s="4"/>
       <c r="D12" s="19" t="s">
@@ -1355,7 +1355,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="18" customHeight="1">
       <c r="A1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="14.25" thickBot="1">

</xml_diff>